<commit_message>
Remove Fields Charge Catalog
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.Catalogue/eFMS.API.Catalogue/Resources/Files/ChargeImportTemplate.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.Catalogue/eFMS.API.Catalogue/Resources/Files/ChargeImportTemplate.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\efms\src\WebAPI\eFMS.API.SystemWeb\CatalogueManagement\eFMS.API.Catalogue\Resources\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\intern.lth002\Desktop\eFMS-WebApp\WebAPI\eFMS.API.SystemWeb\eFMS.API.Catalogue\eFMS.API.Catalogue\Resources\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
   <si>
     <t>DEBIT</t>
   </si>
@@ -48,9 +48,6 @@
     <t>the 11</t>
   </si>
   <si>
-    <t>CRCC-108</t>
-  </si>
-  <si>
     <t>2019Test12</t>
   </si>
   <si>
@@ -96,31 +93,31 @@
     <t>Name Local(*)</t>
   </si>
   <si>
-    <t>Unit(*)</t>
-  </si>
-  <si>
     <t>HAWB</t>
   </si>
   <si>
-    <t>Unit Price(*)</t>
-  </si>
-  <si>
-    <t>Currency(*)</t>
-  </si>
-  <si>
-    <t>VAT(*)</t>
-  </si>
-  <si>
     <t>Type(*)</t>
   </si>
   <si>
     <t>Service(*)</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Unit Price</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>VAT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -479,56 +476,56 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.1796875" customWidth="1"/>
-    <col min="2" max="2" width="17.7265625" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="18.453125" customWidth="1"/>
-    <col min="5" max="5" width="16.453125" customWidth="1"/>
-    <col min="6" max="6" width="17.26953125" customWidth="1"/>
-    <col min="7" max="7" width="16.7265625" customWidth="1"/>
-    <col min="8" max="8" width="14.453125" customWidth="1"/>
-    <col min="9" max="9" width="14.1796875" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="D1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="I1" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -538,18 +535,10 @@
       <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="1">
-        <v>100000</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="1">
-        <v>9029</v>
-      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="1"/>
       <c r="H2" s="1" t="s">
         <v>0</v>
       </c>
@@ -560,24 +549,24 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E3" s="1">
         <v>100000</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G3" s="1">
         <v>9030</v>
@@ -592,24 +581,24 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E4" s="1">
         <v>100000</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G4" s="1">
         <v>9031</v>
@@ -624,24 +613,24 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="D5" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E5" s="1">
         <v>100000</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G5" s="1">
         <v>9032</v>
@@ -668,7 +657,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>